<commit_message>
Base model and template
</commit_message>
<xml_diff>
--- a/data_hsn/interactions.xlsx
+++ b/data_hsn/interactions.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -221,8 +216,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,6 +472,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -486,11 +486,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -561,7 +556,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,10 +588,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -628,7 +622,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -804,14 +797,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="AD16" sqref="AD16"/>
+      <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
@@ -840,74 +833,74 @@
     <col min="25" max="25" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B1" s="28" t="s">
+    <row r="1" spans="1:35">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-    </row>
-    <row r="2" spans="1:35" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="29" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+    </row>
+    <row r="2" spans="1:35" ht="28.9" customHeight="1">
+      <c r="B2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="O2" s="29" t="s">
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="O2" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="30" t="s">
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="30"/>
-      <c r="U2" s="30" t="s">
+      <c r="S2" s="35"/>
+      <c r="U2" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="30"/>
+      <c r="V2" s="35"/>
       <c r="W2" s="16" t="s">
         <v>28</v>
       </c>
@@ -936,7 +929,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35">
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1009,14 +1002,14 @@
       <c r="Y3" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="Z3" s="34" t="s">
+      <c r="Z3" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="AA3" s="35" t="s">
+      <c r="AA3" s="32" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1040,10 +1033,10 @@
       <c r="M4" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="N4" s="31" t="s">
+      <c r="N4" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="31" t="s">
+      <c r="O4" s="28" t="s">
         <v>51</v>
       </c>
       <c r="P4" s="27" t="s">
@@ -1083,7 +1076,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1107,10 +1100,10 @@
       <c r="M5" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="N5" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="O5" s="31" t="s">
+      <c r="O5" s="28" t="s">
         <v>51</v>
       </c>
       <c r="P5" s="27" t="s">
@@ -1150,7 +1143,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1174,10 +1167,10 @@
       <c r="M6" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="31" t="s">
+      <c r="O6" s="28" t="s">
         <v>51</v>
       </c>
       <c r="P6" s="27" t="s">
@@ -1192,32 +1185,32 @@
       <c r="S6" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="T6" s="31" t="s">
+      <c r="T6" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="U6" s="31" t="s">
+      <c r="U6" s="28" t="s">
         <v>46</v>
       </c>
       <c r="V6" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="W6" s="31" t="s">
+      <c r="W6" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="X6" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y6" s="31" t="s">
+      <c r="X6" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y6" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="Z6" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA6" s="31" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="Z6" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA6" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1241,10 +1234,10 @@
       <c r="M7" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="N7" s="31" t="s">
+      <c r="N7" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="31" t="s">
+      <c r="O7" s="28" t="s">
         <v>51</v>
       </c>
       <c r="P7" s="27" t="s">
@@ -1253,38 +1246,38 @@
       <c r="Q7" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="R7" s="31" t="s">
+      <c r="R7" s="28" t="s">
         <v>53</v>
       </c>
       <c r="S7" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="T7" s="31" t="s">
+      <c r="T7" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="U7" s="31" t="s">
+      <c r="U7" s="28" t="s">
         <v>46</v>
       </c>
       <c r="V7" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="W7" s="31" t="s">
+      <c r="W7" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="X7" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y7" s="31" t="s">
+      <c r="X7" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y7" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="Z7" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA7" s="31" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="Z7" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA7" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1308,10 +1301,10 @@
       <c r="M8" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="N8" s="31" t="s">
+      <c r="N8" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="O8" s="31" t="s">
+      <c r="O8" s="28" t="s">
         <v>51</v>
       </c>
       <c r="P8" s="27" t="s">
@@ -1320,38 +1313,38 @@
       <c r="Q8" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="R8" s="31" t="s">
+      <c r="R8" s="28" t="s">
         <v>53</v>
       </c>
       <c r="S8" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="T8" s="31" t="s">
+      <c r="T8" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="U8" s="31" t="s">
+      <c r="U8" s="28" t="s">
         <v>46</v>
       </c>
       <c r="V8" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="W8" s="31" t="s">
+      <c r="W8" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="X8" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y8" s="31" t="s">
+      <c r="X8" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="Z8" s="31" t="s">
+      <c r="Z8" s="28" t="s">
         <v>44</v>
       </c>
       <c r="AA8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1375,10 +1368,10 @@
       <c r="M9" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="N9" s="31" t="s">
+      <c r="N9" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="O9" s="31" t="s">
+      <c r="O9" s="28" t="s">
         <v>51</v>
       </c>
       <c r="P9" s="27" t="s">
@@ -1387,38 +1380,38 @@
       <c r="Q9" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="R9" s="31" t="s">
+      <c r="R9" s="28" t="s">
         <v>53</v>
       </c>
       <c r="S9" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="T9" s="31" t="s">
+      <c r="T9" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="U9" s="31" t="s">
+      <c r="U9" s="28" t="s">
         <v>46</v>
       </c>
       <c r="V9" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="W9" s="31" t="s">
+      <c r="W9" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="X9" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y9" s="31" t="s">
+      <c r="X9" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y9" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="Z9" s="31" t="s">
+      <c r="Z9" s="28" t="s">
         <v>44</v>
       </c>
       <c r="AA9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1442,10 +1435,10 @@
       <c r="M10" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="N10" s="31" t="s">
+      <c r="N10" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="O10" s="31" t="s">
+      <c r="O10" s="28" t="s">
         <v>51</v>
       </c>
       <c r="P10" s="27" t="s">
@@ -1454,38 +1447,38 @@
       <c r="Q10" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="R10" s="31" t="s">
+      <c r="R10" s="28" t="s">
         <v>53</v>
       </c>
       <c r="S10" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="T10" s="31" t="s">
+      <c r="T10" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="U10" s="31" t="s">
+      <c r="U10" s="28" t="s">
         <v>46</v>
       </c>
       <c r="V10" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="W10" s="31" t="s">
+      <c r="W10" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="X10" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y10" s="31" t="s">
+      <c r="X10" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y10" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="Z10" s="31" t="s">
+      <c r="Z10" s="28" t="s">
         <v>44</v>
       </c>
       <c r="AA10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1509,10 +1502,10 @@
       <c r="M11" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="N11" s="31" t="s">
+      <c r="N11" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="O11" s="31" t="s">
+      <c r="O11" s="28" t="s">
         <v>51</v>
       </c>
       <c r="P11" s="27" t="s">
@@ -1521,38 +1514,38 @@
       <c r="Q11" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="R11" s="31" t="s">
+      <c r="R11" s="28" t="s">
         <v>53</v>
       </c>
       <c r="S11" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="T11" s="31" t="s">
+      <c r="T11" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="U11" s="31" t="s">
+      <c r="U11" s="28" t="s">
         <v>46</v>
       </c>
       <c r="V11" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="W11" s="31" t="s">
+      <c r="W11" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="X11" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y11" s="31" t="s">
+      <c r="X11" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y11" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="Z11" s="31" t="s">
+      <c r="Z11" s="28" t="s">
         <v>44</v>
       </c>
       <c r="AA11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1584,7 +1577,7 @@
       <c r="U12" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="V12" s="31" t="s">
+      <c r="V12" s="28" t="s">
         <v>47</v>
       </c>
       <c r="W12" t="s">
@@ -1596,14 +1589,14 @@
       <c r="Y12" t="s">
         <v>34</v>
       </c>
-      <c r="Z12" s="31" t="s">
+      <c r="Z12" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="AA12" s="31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AA12" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1629,7 +1622,7 @@
       <c r="U13" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="V13" s="31" t="s">
+      <c r="V13" s="28" t="s">
         <v>47</v>
       </c>
       <c r="W13" t="s">
@@ -1641,14 +1634,14 @@
       <c r="Y13" t="s">
         <v>34</v>
       </c>
-      <c r="Z13" s="31" t="s">
+      <c r="Z13" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="AA13" s="31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AA13" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1674,7 +1667,7 @@
       <c r="U14" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="V14" s="31" t="s">
+      <c r="V14" s="28" t="s">
         <v>47</v>
       </c>
       <c r="W14" t="s">
@@ -1686,14 +1679,14 @@
       <c r="Y14" t="s">
         <v>34</v>
       </c>
-      <c r="Z14" s="31" t="s">
+      <c r="Z14" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="AA14" s="31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AA14" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1719,7 +1712,7 @@
       <c r="U15" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="V15" s="31" t="s">
+      <c r="V15" s="28" t="s">
         <v>47</v>
       </c>
       <c r="W15" t="s">
@@ -1731,46 +1724,46 @@
       <c r="Y15" t="s">
         <v>34</v>
       </c>
-      <c r="Z15" s="31" t="s">
+      <c r="Z15" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="AA15" s="31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+      <c r="AA15" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="30">
       <c r="A16" s="8" t="s">
         <v>16</v>
       </c>
       <c r="N16" s="2"/>
-      <c r="O16" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="P16" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q16" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="R16" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="S16" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="T16" s="32" t="s">
+      <c r="O16" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="P16" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q16" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="R16" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="S16" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="T16" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="U16" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="V16" s="31" t="s">
+      <c r="U16" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="V16" s="28" t="s">
         <v>55</v>
       </c>
       <c r="W16" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="X16" s="33" t="s">
+      <c r="X16" s="30" t="s">
         <v>44</v>
       </c>
       <c r="Y16" s="27" t="s">
@@ -1783,7 +1776,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27">
       <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
@@ -1802,7 +1795,7 @@
       <c r="U17" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="V17" s="31" t="s">
+      <c r="V17" s="28" t="s">
         <v>53</v>
       </c>
       <c r="W17" s="27" t="s">
@@ -1821,7 +1814,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27">
       <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
@@ -1839,7 +1832,7 @@
       <c r="U18" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="V18" s="31" t="s">
+      <c r="V18" s="28" t="s">
         <v>53</v>
       </c>
       <c r="X18" s="21" t="s">
@@ -1849,7 +1842,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27">
       <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
@@ -1866,7 +1859,7 @@
       <c r="U19" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="V19" s="31" t="s">
+      <c r="V19" s="28" t="s">
         <v>53</v>
       </c>
       <c r="X19" t="s">
@@ -1876,7 +1869,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
@@ -1891,7 +1884,7 @@
       <c r="U20" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="V20" s="31" t="s">
+      <c r="V20" s="28" t="s">
         <v>55</v>
       </c>
       <c r="W20" s="27" t="s">
@@ -1910,7 +1903,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27">
       <c r="A21" s="12" t="s">
         <v>21</v>
       </c>
@@ -1922,7 +1915,7 @@
       <c r="U21" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="V21" s="31" t="s">
+      <c r="V21" s="28" t="s">
         <v>55</v>
       </c>
       <c r="X21" t="s">
@@ -1932,7 +1925,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27">
       <c r="A22" s="19" t="s">
         <v>26</v>
       </c>
@@ -1956,7 +1949,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27">
       <c r="A23" s="17" t="s">
         <v>30</v>
       </c>
@@ -1975,7 +1968,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27">
       <c r="A24" s="17" t="s">
         <v>27</v>
       </c>
@@ -1996,7 +1989,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27">
       <c r="A25" s="18" t="s">
         <v>29</v>
       </c>
@@ -2014,7 +2007,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27">
       <c r="A26" s="22" t="s">
         <v>31</v>
       </c>
@@ -2029,7 +2022,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27">
       <c r="A27" s="23" t="s">
         <v>32</v>
       </c>
@@ -2041,8 +2034,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+    <row r="28" spans="1:27">
+      <c r="A28" s="31" t="s">
         <v>37</v>
       </c>
       <c r="Z28" s="2"/>
@@ -2050,8 +2043,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+    <row r="29" spans="1:27">
+      <c r="A29" s="32" t="s">
         <v>39</v>
       </c>
       <c r="AA29" s="2"/>
@@ -2071,24 +2064,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>